<commit_message>
Seperating faceplates and Flex Boxes/Tubes.
CSV/mkcsv.py is now doing the following:
- Seperating OCS Faceplates (for boxes) and Flex Tubes
- Pulling in the serials and earliest dates from the Flex.FlesHist table
- Creating individual histories of OCS Flex controllers

CPU/Makefile has updated references for files
CPU/mksql.py had the fetch_ocs method removed, it was moved to CPU/mkcsv.py

Updated source Excel files. Removed references to old directories that have
been removed.

Patrick provided FlexComponentsTracking as a Iridium SIM reference;
Already had it in here, but added it for tracking purposes.
</commit_message>
<xml_diff>
--- a/TFLEX_TEST_LOG.xlsx
+++ b/TFLEX_TEST_LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/white/Repos/Dev/dbFlexControllers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7319F8-2CA8-CE46-B9EF-8427F85ABCBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDEBE5B-5CA4-2F4A-955B-1D057B20C45D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34140" windowHeight="28240" tabRatio="756" firstSheet="60" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17060" yWindow="460" windowWidth="34140" windowHeight="28240" tabRatio="756" firstSheet="60" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0000" sheetId="2" r:id="rId1"/>
@@ -16560,7 +16560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed scraping of data, moved to UX dev.
Pulling in and using as much data as possible from the given sources. 
Have this up and running in the prefixed test database currently.
</commit_message>
<xml_diff>
--- a/TFLEX_TEST_LOG.xlsx
+++ b/TFLEX_TEST_LOG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/white/Repos/Dev/dbFlexControllers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55210814-714E-4C4F-B70A-B9CB9C74453E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14960A2-5E58-6546-859D-EE37A4D084CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34140" windowHeight="28240" tabRatio="756" firstSheet="58" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34140" windowHeight="28240" tabRatio="756" firstSheet="44" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0000" sheetId="2" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="1092">
   <si>
     <t>SSTC=OK, TESTIND=OK, ATRH=ON, WIND=OK, SWR=OK, RAIN=OK  -jms</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3202,9 +3202,6 @@
     <t>Updated firmware to version 2.01, 170530.</t>
   </si>
   <si>
-    <t>Used for Grassy Knoll testing</t>
-  </si>
-  <si>
     <t>Updated Iridium 1st Xmit time to 00:40.</t>
   </si>
   <si>
@@ -3298,9 +3295,6 @@
     <t>Ryan says Iridium now not working??? Needs testing???</t>
   </si>
   <si>
-    <t>Iridium needs to be checked out, Ryan says bad.</t>
-  </si>
-  <si>
     <t>Ran this system an additional 6 days, and it did NOT have any additonal resets, so I think its okay, and may have been an issue with just one of the Iridium 6 hour buffer transmits.</t>
   </si>
   <si>
@@ -3355,9 +3349,6 @@
     <t>Installed Iridium SIM card.</t>
   </si>
   <si>
-    <t>Ran Bench current drain test for  7 days with version 2.01, 170530 firmware, RF modem turned off, 14.25mA Average. Downloaded and checked Flash RAM data, which looked good.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> indicates current drain test run with Gill Wind sensor with NEW Ocean Server 4000T compass, starting 8/7/2018.</t>
   </si>
   <si>
@@ -3374,6 +3365,51 @@
   </si>
   <si>
     <t>Ran Bench current drain test for  3.5 days with version 2.01, 170530 firmware, RF modem turned off, 13.84mA Average. Downloaded and checked Flash RAM data, which looked good.</t>
+  </si>
+  <si>
+    <t>Gave to Patrick for TELOS testing</t>
+  </si>
+  <si>
+    <t>Back from Indonesia, IO1-18, not deployed.</t>
+  </si>
+  <si>
+    <t>Back from Indonesia, IO1-18.  NEEDS TESTING, REPAIR for GPS, GPS module on RIG board? Or NEW GPS antenna???</t>
+  </si>
+  <si>
+    <t>Back from Indonesia, IO1-18, NOT deployed, needs checkout/upgrades.</t>
+  </si>
+  <si>
+    <t>Ran Bench current drain test for 3 days with version 2.01, 170530 firmware, RF modem turned off, 13.23mA Average. Downloaded and checked Flash RAM data, which looked good.</t>
+  </si>
+  <si>
+    <t>Installed metal SS standoffs on bottom of circuit board stack.</t>
+  </si>
+  <si>
+    <t>Back from IO2-18-RB, NOT USED, not deployed at 12S-67E due to bad weather on site.</t>
+  </si>
+  <si>
+    <t>Ran Bench current drain test for 4 days with version 2.01, 170530 firmware, RF modem turned off, 12.99mA Average.</t>
+  </si>
+  <si>
+    <t>Successfully tested GPS and XMIT commands outside on the internal antennas.</t>
+  </si>
+  <si>
+    <t>Installed metal SS standoffs on the bottom of the circuit board stack.</t>
+  </si>
+  <si>
+    <t>Back from IO2-18-RB, not deployed at 8S-81E due to bad weather.</t>
+  </si>
+  <si>
+    <t>Back from IO2-18-RB, not deployed due to rough weather</t>
+  </si>
+  <si>
+    <t>Ran 3 day current drain test, everything worked okay, 12.63mA average.</t>
+  </si>
+  <si>
+    <t>Ran Current drain test for 4 days, 12.88 mA Average.  Dumped FLASH RAM data file, which looked okay.</t>
+  </si>
+  <si>
+    <t>Successfully tested GPS and Iridium XMIT commands outside with internal antennas.</t>
   </si>
 </sst>
 </file>
@@ -4918,7 +4954,7 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="55" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -4927,7 +4963,7 @@
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="29" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -4936,7 +4972,7 @@
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="29" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
@@ -5827,7 +5863,7 @@
         <v>43182</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -5835,7 +5871,7 @@
         <v>43334</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -5844,7 +5880,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="32" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -5853,7 +5889,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="32" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="42" x14ac:dyDescent="0.15">
@@ -5862,7 +5898,7 @@
       </c>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -5871,7 +5907,7 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="32" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -5880,7 +5916,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="11" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="42" x14ac:dyDescent="0.15">
@@ -5889,14 +5925,14 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="11" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="11" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="56" x14ac:dyDescent="0.15">
@@ -5905,7 +5941,7 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="32" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -5914,7 +5950,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="32" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
@@ -6803,7 +6839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="150" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
@@ -7563,7 +7599,7 @@
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="11" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.15">
@@ -8568,10 +8604,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8673,17 +8709,29 @@
         <v>871</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="2"/>
-      <c r="C13" s="11"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="2"/>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="2"/>
-      <c r="C15" s="11"/>
+    <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="6">
+        <v>43363</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="6">
+        <v>43409</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="6">
+        <v>43413</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>1089</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
@@ -8711,9 +8759,6 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8843,10 +8888,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8904,7 +8949,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <v>43083</v>
       </c>
       <c r="C7" s="32" t="s">
@@ -8912,21 +8957,44 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>43084</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="2"/>
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="6">
+        <v>43363</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="6">
+        <v>43412</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="6">
+        <v>43417</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="6">
+        <v>43417</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>1091</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
@@ -8966,6 +9034,12 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9464,7 +9538,7 @@
         <v>43252</v>
       </c>
       <c r="C8" s="60" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -9472,7 +9546,7 @@
         <v>43327</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -9480,7 +9554,7 @@
         <v>43327</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -9488,7 +9562,7 @@
         <v>43327</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -9496,7 +9570,7 @@
         <v>43339</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -9504,7 +9578,7 @@
         <v>43339</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -9512,7 +9586,7 @@
         <v>43339</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -11139,7 +11213,7 @@
         <v>43252</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11147,7 +11221,7 @@
         <v>43325</v>
       </c>
       <c r="C8" s="60" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11155,7 +11229,7 @@
         <v>43325</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11163,7 +11237,7 @@
         <v>43325</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11171,7 +11245,7 @@
         <v>43332</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11179,7 +11253,7 @@
         <v>43332</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11187,7 +11261,7 @@
         <v>43332</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -11285,7 +11359,7 @@
         <v>43252</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11293,7 +11367,7 @@
         <v>43319</v>
       </c>
       <c r="C8" s="60" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11301,7 +11375,7 @@
         <v>43319</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11309,7 +11383,7 @@
         <v>43319</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11317,7 +11391,7 @@
         <v>43326</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11325,7 +11399,7 @@
         <v>43326</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -11333,7 +11407,7 @@
         <v>43326</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -13444,7 +13518,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13516,9 +13590,13 @@
         <v>980</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="6"/>
-      <c r="C9" s="60"/>
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="6">
+        <v>43403</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>1079</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="6"/>
@@ -13752,8 +13830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="C24" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="C27" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14074,9 +14152,13 @@
         <v>812</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="2"/>
-      <c r="C36" s="8"/>
+    <row r="36" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A36" s="6">
+        <v>43403</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>1078</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C37" s="8"/>
@@ -14094,7 +14176,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14167,9 +14249,13 @@
         <v>805</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="6"/>
-      <c r="C9" s="60"/>
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="6">
+        <v>43403</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>1080</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="6"/>
@@ -14570,10 +14656,10 @@
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14645,20 +14731,37 @@
         <v>861</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="6"/>
-      <c r="C9" s="60"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" s="6"/>
-      <c r="C10" s="60"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="6"/>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="2"/>
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="6">
+        <v>43358</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="6">
+        <v>43405</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="6">
+        <v>43409</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="6">
+        <v>43409</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>1085</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
@@ -14713,6 +14816,9 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16027,7 +16133,7 @@
         <v>43319</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -16134,7 +16240,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C1" s="11"/>
     </row>
@@ -16158,7 +16264,7 @@
       </c>
       <c r="B4" s="64"/>
       <c r="C4" s="32" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -16176,7 +16282,7 @@
       </c>
       <c r="B6" s="64"/>
       <c r="C6" s="32" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -16184,7 +16290,7 @@
         <v>43363</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -16192,7 +16298,7 @@
         <v>43398</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -16200,7 +16306,7 @@
         <v>43398</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -16299,7 +16405,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C1" s="11"/>
     </row>
@@ -16323,7 +16429,7 @@
       </c>
       <c r="B4" s="64"/>
       <c r="C4" s="32" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -16341,7 +16447,7 @@
       </c>
       <c r="B6" s="64"/>
       <c r="C6" s="32" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -16349,7 +16455,7 @@
         <v>43402</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -16456,7 +16562,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C1" s="11"/>
     </row>
@@ -16480,7 +16586,7 @@
       </c>
       <c r="B4" s="64"/>
       <c r="C4" s="32" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -16498,17 +16604,21 @@
       </c>
       <c r="B6" s="64"/>
       <c r="C6" s="32" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6">
+        <v>43405</v>
+      </c>
       <c r="C7" s="32" t="s">
-        <v>1073</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6">
+        <v>43405</v>
+      </c>
       <c r="C8" s="32" t="s">
         <v>1011</v>
       </c>
@@ -17889,19 +17999,19 @@
     </row>
     <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A66" s="61" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B66" s="74">
         <v>1061</v>
       </c>
       <c r="C66" s="76" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="D66" s="61" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E66" s="77" t="s">
         <v>1062</v>
-      </c>
-      <c r="E66" s="77" t="s">
-        <v>1064</v>
       </c>
       <c r="F66" s="75">
         <v>43355</v>
@@ -17909,19 +18019,19 @@
     </row>
     <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A67" s="61" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B67" s="74">
         <v>1062</v>
       </c>
       <c r="C67" s="76" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="D67" s="61" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E67" s="77" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="F67" s="75">
         <v>43355</v>
@@ -17929,19 +18039,19 @@
     </row>
     <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A68" s="61" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B68" s="74">
         <v>1063</v>
       </c>
       <c r="C68" s="76" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="D68" s="61" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E68" s="77" t="s">
         <v>1067</v>
-      </c>
-      <c r="E68" s="77" t="s">
-        <v>1069</v>
       </c>
       <c r="F68" s="75">
         <v>43355</v>
@@ -17961,8 +18071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView topLeftCell="A8" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18071,7 +18181,7 @@
         <v>159</v>
       </c>
       <c r="J4" s="57" t="s">
-        <v>1022</v>
+        <v>1077</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>177</v>
@@ -18923,7 +19033,7 @@
         <v>159</v>
       </c>
       <c r="J21" s="28" t="s">
-        <v>1054</v>
+        <v>1077</v>
       </c>
       <c r="K21" s="48" t="s">
         <v>417</v>
@@ -19087,7 +19197,9 @@
       <c r="P24" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="Q24" s="3"/>
+      <c r="Q24" s="3" t="s">
+        <v>400</v>
+      </c>
       <c r="R24" s="52" t="s">
         <v>514</v>
       </c>
@@ -19185,7 +19297,9 @@
       <c r="P26" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="Q26" s="3"/>
+      <c r="Q26" s="30" t="s">
+        <v>400</v>
+      </c>
       <c r="R26" s="52" t="s">
         <v>548</v>
       </c>
@@ -20599,7 +20713,9 @@
       <c r="P57" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="Q57" s="3"/>
+      <c r="Q57" s="3" t="s">
+        <v>400</v>
+      </c>
       <c r="R57" s="52" t="s">
         <v>827</v>
       </c>
@@ -20922,7 +21038,7 @@
     </row>
     <row r="65" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="52" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B65" s="3">
         <v>1061</v>
@@ -20942,7 +21058,7 @@
       </c>
       <c r="J65" s="28"/>
       <c r="K65" s="48" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="L65" s="30" t="s">
         <v>298</v>
@@ -20963,12 +21079,12 @@
         <v>400</v>
       </c>
       <c r="R65" s="52" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="52" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B66" s="3">
         <v>1062</v>
@@ -20988,7 +21104,7 @@
       </c>
       <c r="J66" s="28"/>
       <c r="K66" s="48" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="L66" s="30" t="s">
         <v>298</v>
@@ -21009,12 +21125,12 @@
         <v>400</v>
       </c>
       <c r="R66" s="52" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="67" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A67" s="52" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B67" s="3">
         <v>1063</v>
@@ -21034,7 +21150,7 @@
       </c>
       <c r="J67" s="28"/>
       <c r="K67" s="48" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="L67" s="30" t="s">
         <v>298</v>
@@ -21055,7 +21171,7 @@
         <v>400</v>
       </c>
       <c r="R67" s="52" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
   </sheetData>
@@ -21073,8 +21189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21110,7 +21226,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="35" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
@@ -21125,7 +21241,7 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="110"/>
       <c r="B5" s="35" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="C5" s="35"/>
     </row>
@@ -21633,6 +21749,12 @@
       <c r="E28" s="38">
         <v>13.55</v>
       </c>
+      <c r="F28" s="108">
+        <v>43413</v>
+      </c>
+      <c r="G28" s="109">
+        <v>12.63</v>
+      </c>
     </row>
     <row r="29" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="36" t="s">
@@ -21661,6 +21783,12 @@
       <c r="E30" s="38">
         <v>13.75</v>
       </c>
+      <c r="F30" s="108">
+        <v>43417</v>
+      </c>
+      <c r="G30" s="109">
+        <v>12.88</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="36" t="s">
@@ -22069,6 +22197,12 @@
       <c r="C60" s="34">
         <v>13.62</v>
       </c>
+      <c r="D60" s="108">
+        <v>43409</v>
+      </c>
+      <c r="E60" s="109">
+        <v>12.99</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="78" t="s">
@@ -22155,7 +22289,7 @@
     </row>
     <row r="68" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="36" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B68" s="108">
         <v>43398</v>
@@ -22166,7 +22300,7 @@
     </row>
     <row r="69" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="36" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B69" s="108">
         <v>43402</v>
@@ -22177,10 +22311,14 @@
     </row>
     <row r="70" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A70" s="36" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B70" s="115"/>
-      <c r="C70" s="115"/>
+        <v>1047</v>
+      </c>
+      <c r="B70" s="108">
+        <v>43405</v>
+      </c>
+      <c r="C70" s="115">
+        <v>13.23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Installed from this commit. DO NOT CHANGE.
Installed data from this commit. No further addtions, deletions, or changes.
</commit_message>
<xml_diff>
--- a/TFLEX_TEST_LOG.xlsx
+++ b/TFLEX_TEST_LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/white/Repos/Dev/dbFlexControllers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71F1527-0B83-2F44-AE17-183F94B86403}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4EC351-0E59-4143-8AC3-D1532F04F343}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17060" yWindow="460" windowWidth="34140" windowHeight="28340" tabRatio="756" firstSheet="44" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2256" uniqueCount="1143">
   <si>
     <t>SSTC=OK, TESTIND=OK, ATRH=ON, WIND=OK, SWR=OK, RAIN=OK  -jms</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3539,9 +3539,6 @@
     <t>Installed NEW face and jam seal O-rings.</t>
   </si>
   <si>
-    <t>Installed NEW CPU board.</t>
-  </si>
-  <si>
     <t>Ran Bench current drain test for 2 days with version 2.01, 170530 firmware, RF modem turned off, 13.04mA Average.</t>
   </si>
   <si>
@@ -3549,6 +3546,24 @@
   </si>
   <si>
     <t>INSTALLED NEW CPU BOARD with 2.01, 170530, and new 2 GB FLASH RAM card.</t>
+  </si>
+  <si>
+    <t>Ran Current drain BENCH test for 3 days, 13.26mA Average.  Dumped FLASH RAM data file, which looked okay.</t>
+  </si>
+  <si>
+    <t>Installed NEW CPU board with firmware v2.01, 170530.</t>
+  </si>
+  <si>
+    <t>Successfully tested GPS and XMIT commands outside on internal antennas.</t>
+  </si>
+  <si>
+    <t>Rec RT015, 4S67E, IO2-18-RB, WIND CH BAD?</t>
+  </si>
+  <si>
+    <t>Back from IO2-18-RB.  Rec RT015, 4S67E.  On the shelf, waiting for post deploy testing/upgrades.  Gill WIND data failed during deployment, went to 1E+35CH.  TFLEX wind channel needs testing, BAD?  Gill wind sn16100041 calibrated okay, wind and compass cals?</t>
+  </si>
+  <si>
+    <t>From TFLEX DATA "System Status":  "All anemometer (Gill Windsonic #16100041) data become 1E+35. Compass data OK"</t>
   </si>
 </sst>
 </file>
@@ -3691,7 +3706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4041,6 +4056,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9453,10 +9471,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9545,7 +9563,7 @@
         <v>43517</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -9580,24 +9598,33 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="C16" s="32"/>
+    <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="6">
+        <v>43521</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>1137</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
+      <c r="A17" s="6">
+        <v>43521</v>
+      </c>
       <c r="C17" s="32" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="6"/>
+      <c r="C18" s="32" t="s">
         <v>1128</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="2"/>
-      <c r="C18" s="32" t="s">
+    <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="2"/>
+      <c r="C19" s="32" t="s">
         <v>1129</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
@@ -9655,6 +9682,9 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12075,7 +12105,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12996,10 +13026,10 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13056,9 +13086,112 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="6">
+        <v>42641</v>
+      </c>
       <c r="C7" s="60" t="s">
         <v>600</v>
       </c>
+    </row>
+    <row r="8" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A8" s="6">
+        <v>43358</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A9" s="6">
+        <v>43521</v>
+      </c>
+      <c r="C9" s="120" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16653,7 +16786,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16746,8 +16879,8 @@
       <c r="A11" s="6">
         <v>43516</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>1134</v>
+      <c r="C11" s="32" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -16755,7 +16888,7 @@
         <v>43518</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -16763,7 +16896,7 @@
         <v>43518</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -18689,8 +18822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A30" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20805,7 +20938,9 @@
       <c r="I44" s="80" t="s">
         <v>715</v>
       </c>
-      <c r="J44" s="28"/>
+      <c r="J44" s="28" t="s">
+        <v>1140</v>
+      </c>
       <c r="K44" s="48" t="s">
         <v>643</v>
       </c>
@@ -21892,8 +22027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -22541,10 +22676,10 @@
         <v>14.23</v>
       </c>
       <c r="D32" s="83">
-        <v>43518</v>
+        <v>43521</v>
       </c>
       <c r="E32" s="84">
-        <v>13.04</v>
+        <v>13.26</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -22989,7 +23124,7 @@
         <v>16.61</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="36" t="s">
         <v>967</v>
       </c>
@@ -23000,7 +23135,7 @@
         <v>14.17</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="36" t="s">
         <v>968</v>
       </c>
@@ -23011,7 +23146,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A67" s="36" t="s">
         <v>969</v>
       </c>
@@ -23027,8 +23162,14 @@
       <c r="E67" s="109">
         <v>12.94</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="F67" s="83">
+        <v>43518</v>
+      </c>
+      <c r="G67" s="84">
+        <v>13.04</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="36" t="s">
         <v>1041</v>
       </c>
@@ -23039,7 +23180,7 @@
         <v>13.33</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="36" t="s">
         <v>1042</v>
       </c>
@@ -23050,7 +23191,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A70" s="36" t="s">
         <v>1043</v>
       </c>

</xml_diff>